<commit_message>
Thêm bốn bài tập excel
</commit_message>
<xml_diff>
--- a/Quiz2__Computer Fundamentals.xlsx
+++ b/Quiz2__Computer Fundamentals.xlsx
@@ -354,7 +354,7 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,6 +382,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -496,7 +502,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -583,25 +589,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -612,6 +599,28 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -862,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z971"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39:K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -1025,10 +1034,10 @@
       <c r="A6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="37"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="8"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1054,13 +1063,13 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="37"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1086,7 +1095,7 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A8" s="39"/>
+      <c r="A8" s="41"/>
       <c r="B8" s="9" t="s">
         <v>7</v>
       </c>
@@ -1118,7 +1127,7 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A9" s="39"/>
+      <c r="A9" s="41"/>
       <c r="B9" s="9" t="s">
         <v>9</v>
       </c>
@@ -1150,7 +1159,7 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A10" s="39"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="9" t="s">
         <v>11</v>
       </c>
@@ -1182,11 +1191,11 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A11" s="40"/>
+      <c r="A11" s="42"/>
       <c r="B11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="36" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="1"/>
@@ -1214,13 +1223,13 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="37"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -1246,7 +1255,7 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A13" s="39"/>
+      <c r="A13" s="41"/>
       <c r="B13" s="9" t="s">
         <v>7</v>
       </c>
@@ -1278,11 +1287,11 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A14" s="39"/>
+      <c r="A14" s="41"/>
       <c r="B14" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="37" t="s">
         <v>18</v>
       </c>
       <c r="D14" s="1"/>
@@ -1310,7 +1319,7 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A15" s="39"/>
+      <c r="A15" s="41"/>
       <c r="B15" s="14" t="s">
         <v>11</v>
       </c>
@@ -1342,7 +1351,7 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A16" s="40"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="14" t="s">
         <v>13</v>
       </c>
@@ -1374,13 +1383,13 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="37"/>
+      <c r="C17" s="44"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1406,7 +1415,7 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A18" s="39"/>
+      <c r="A18" s="41"/>
       <c r="B18" s="14" t="s">
         <v>7</v>
       </c>
@@ -1438,11 +1447,11 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="33.75" customHeight="1">
-      <c r="A19" s="39"/>
+      <c r="A19" s="41"/>
       <c r="B19" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="47" t="s">
+      <c r="C19" s="38" t="s">
         <v>24</v>
       </c>
       <c r="D19" s="1"/>
@@ -1470,7 +1479,7 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A20" s="39"/>
+      <c r="A20" s="41"/>
       <c r="B20" s="14" t="s">
         <v>11</v>
       </c>
@@ -1502,7 +1511,7 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A21" s="40"/>
+      <c r="A21" s="42"/>
       <c r="B21" s="14" t="s">
         <v>13</v>
       </c>
@@ -1534,13 +1543,13 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="37"/>
+      <c r="C22" s="44"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -1566,11 +1575,11 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" ht="44.25" customHeight="1">
-      <c r="A23" s="39"/>
+      <c r="A23" s="41"/>
       <c r="B23" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="47" t="s">
+      <c r="C23" s="38" t="s">
         <v>29</v>
       </c>
       <c r="D23" s="1"/>
@@ -1598,7 +1607,7 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A24" s="39"/>
+      <c r="A24" s="41"/>
       <c r="B24" s="14" t="s">
         <v>9</v>
       </c>
@@ -1630,7 +1639,7 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A25" s="39"/>
+      <c r="A25" s="41"/>
       <c r="B25" s="14" t="s">
         <v>11</v>
       </c>
@@ -1662,7 +1671,7 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A26" s="40"/>
+      <c r="A26" s="42"/>
       <c r="B26" s="14" t="s">
         <v>13</v>
       </c>
@@ -1694,7 +1703,7 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="40" t="s">
         <v>33</v>
       </c>
       <c r="B27" s="17" t="s">
@@ -1726,11 +1735,11 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A28" s="39"/>
+      <c r="A28" s="41"/>
       <c r="B28" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="48" t="s">
+      <c r="C28" s="39" t="s">
         <v>35</v>
       </c>
       <c r="D28" s="1"/>
@@ -1758,7 +1767,7 @@
       <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A29" s="39"/>
+      <c r="A29" s="41"/>
       <c r="B29" s="12" t="s">
         <v>9</v>
       </c>
@@ -1790,7 +1799,7 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A30" s="39"/>
+      <c r="A30" s="41"/>
       <c r="B30" s="12" t="s">
         <v>11</v>
       </c>
@@ -1822,7 +1831,7 @@
       <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A31" s="40"/>
+      <c r="A31" s="42"/>
       <c r="B31" s="12" t="s">
         <v>13</v>
       </c>
@@ -1854,7 +1863,7 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A32" s="38" t="s">
+      <c r="A32" s="40" t="s">
         <v>39</v>
       </c>
       <c r="B32" s="20" t="s">
@@ -1886,7 +1895,7 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A33" s="39"/>
+      <c r="A33" s="41"/>
       <c r="B33" s="12" t="s">
         <v>7</v>
       </c>
@@ -1918,11 +1927,11 @@
       <c r="Z33" s="1"/>
     </row>
     <row r="34" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A34" s="39"/>
+      <c r="A34" s="41"/>
       <c r="B34" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="46" t="s">
+      <c r="C34" s="49" t="s">
         <v>42</v>
       </c>
       <c r="D34" s="1"/>
@@ -1950,11 +1959,11 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A35" s="39"/>
+      <c r="A35" s="41"/>
       <c r="B35" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="37" t="s">
         <v>43</v>
       </c>
       <c r="D35" s="1"/>
@@ -1982,7 +1991,7 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A36" s="40"/>
+      <c r="A36" s="42"/>
       <c r="B36" s="12" t="s">
         <v>13</v>
       </c>
@@ -2014,7 +2023,7 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A37" s="38" t="s">
+      <c r="A37" s="40" t="s">
         <v>45</v>
       </c>
       <c r="B37" s="17" t="s">
@@ -2046,7 +2055,7 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A38" s="39"/>
+      <c r="A38" s="41"/>
       <c r="B38" s="9" t="s">
         <v>7</v>
       </c>
@@ -2078,11 +2087,11 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A39" s="39"/>
+      <c r="A39" s="41"/>
       <c r="B39" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C39" s="45">
+      <c r="C39" s="36">
         <v>2</v>
       </c>
       <c r="D39" s="1"/>
@@ -2110,7 +2119,7 @@
       <c r="Z39" s="1"/>
     </row>
     <row r="40" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A40" s="39"/>
+      <c r="A40" s="41"/>
       <c r="B40" s="9" t="s">
         <v>11</v>
       </c>
@@ -2142,7 +2151,7 @@
       <c r="Z40" s="1"/>
     </row>
     <row r="41" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A41" s="40"/>
+      <c r="A41" s="42"/>
       <c r="B41" s="9" t="s">
         <v>13</v>
       </c>
@@ -2174,13 +2183,13 @@
       <c r="Z41" s="1"/>
     </row>
     <row r="42" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A42" s="38" t="s">
+      <c r="A42" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="B42" s="41" t="s">
+      <c r="B42" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="37"/>
+      <c r="C42" s="44"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -2206,7 +2215,7 @@
       <c r="Z42" s="1"/>
     </row>
     <row r="43" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A43" s="39"/>
+      <c r="A43" s="41"/>
       <c r="B43" s="9" t="s">
         <v>7</v>
       </c>
@@ -2238,7 +2247,7 @@
       <c r="Z43" s="1"/>
     </row>
     <row r="44" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A44" s="39"/>
+      <c r="A44" s="41"/>
       <c r="B44" s="12" t="s">
         <v>9</v>
       </c>
@@ -2270,7 +2279,7 @@
       <c r="Z44" s="1"/>
     </row>
     <row r="45" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A45" s="39"/>
+      <c r="A45" s="41"/>
       <c r="B45" s="12" t="s">
         <v>11</v>
       </c>
@@ -2302,11 +2311,11 @@
       <c r="Z45" s="1"/>
     </row>
     <row r="46" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A46" s="40"/>
+      <c r="A46" s="42"/>
       <c r="B46" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C46" s="46" t="s">
+      <c r="C46" s="37" t="s">
         <v>52</v>
       </c>
       <c r="D46" s="1"/>
@@ -2334,13 +2343,13 @@
       <c r="Z46" s="1"/>
     </row>
     <row r="47" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A47" s="38" t="s">
+      <c r="A47" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="B47" s="42" t="s">
+      <c r="B47" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="C47" s="37"/>
+      <c r="C47" s="44"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -2366,7 +2375,7 @@
       <c r="Z47" s="1"/>
     </row>
     <row r="48" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A48" s="39"/>
+      <c r="A48" s="41"/>
       <c r="B48" s="12" t="s">
         <v>7</v>
       </c>
@@ -2398,7 +2407,7 @@
       <c r="Z48" s="1"/>
     </row>
     <row r="49" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A49" s="39"/>
+      <c r="A49" s="41"/>
       <c r="B49" s="12" t="s">
         <v>9</v>
       </c>
@@ -2430,7 +2439,7 @@
       <c r="Z49" s="1"/>
     </row>
     <row r="50" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A50" s="39"/>
+      <c r="A50" s="41"/>
       <c r="B50" s="12" t="s">
         <v>11</v>
       </c>
@@ -2462,11 +2471,11 @@
       <c r="Z50" s="1"/>
     </row>
     <row r="51" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A51" s="40"/>
+      <c r="A51" s="42"/>
       <c r="B51" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C51" s="46">
+      <c r="C51" s="37">
         <v>4</v>
       </c>
       <c r="D51" s="1"/>
@@ -2494,13 +2503,13 @@
       <c r="Z51" s="1"/>
     </row>
     <row r="52" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A52" s="38" t="s">
+      <c r="A52" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="B52" s="43" t="s">
+      <c r="B52" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="C52" s="44"/>
+      <c r="C52" s="46"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -2526,7 +2535,7 @@
       <c r="Z52" s="1"/>
     </row>
     <row r="53" spans="1:26" ht="28.5" customHeight="1">
-      <c r="A53" s="39"/>
+      <c r="A53" s="41"/>
       <c r="B53" s="12" t="s">
         <v>7</v>
       </c>
@@ -2558,7 +2567,7 @@
       <c r="Z53" s="1"/>
     </row>
     <row r="54" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A54" s="39"/>
+      <c r="A54" s="41"/>
       <c r="B54" s="12" t="s">
         <v>9</v>
       </c>
@@ -2590,7 +2599,7 @@
       <c r="Z54" s="1"/>
     </row>
     <row r="55" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A55" s="39"/>
+      <c r="A55" s="41"/>
       <c r="B55" s="12" t="s">
         <v>11</v>
       </c>
@@ -2622,11 +2631,11 @@
       <c r="Z55" s="1"/>
     </row>
     <row r="56" spans="1:26" ht="19.5" customHeight="1">
-      <c r="A56" s="40"/>
+      <c r="A56" s="42"/>
       <c r="B56" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C56" s="46" t="s">
+      <c r="C56" s="37" t="s">
         <v>52</v>
       </c>
       <c r="D56" s="1"/>
@@ -28275,6 +28284,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:C12"/>
     <mergeCell ref="A17:A21"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="A47:A51"/>
@@ -28288,11 +28302,6 @@
     <mergeCell ref="A37:A41"/>
     <mergeCell ref="A42:A46"/>
     <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <phoneticPr fontId="13"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>